<commit_message>
Version 1.5.0 : Updated Backend and excel template for water leaktest changes, and improved login message alert
</commit_message>
<xml_diff>
--- a/excel_import/water_leaktest_report_template.xlsx
+++ b/excel_import/water_leaktest_report_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="265" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B1853AE-08E0-4263-B286-3A80E6280B58}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8528651E-2C1C-42FE-9717-D837F7F868D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1575" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Part Number :</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>Water Leaktest Result Report</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -198,23 +201,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -239,27 +239,24 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -292,9 +289,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -332,7 +329,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -438,7 +435,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -580,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -591,33 +588,30 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L11"/>
+  <dimension ref="B1:M11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="22" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="25" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="25" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" style="26" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" style="21" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="21" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="21" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="22" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="1" width="5.140625" style="18" customWidth="1"/>
+    <col min="2" max="3" width="22.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="21" customWidth="1"/>
+    <col min="7" max="8" width="21.85546875" style="21" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="21" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" style="22" customWidth="1"/>
+    <col min="11" max="11" width="22.140625" style="17" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" style="17" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" style="17" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="18" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="4"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="4"/>
+    <row r="1" spans="2:13" s="1" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -625,85 +619,88 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" spans="2:12" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+      <c r="L1" s="2"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="2:13" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
-    </row>
-    <row r="3" spans="2:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="2:13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="5"/>
-    </row>
-    <row r="4" spans="2:12" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="C3" s="10"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="2:13" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="5"/>
-    </row>
-    <row r="5" spans="2:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="J4" s="2"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="L5" s="13"/>
-    </row>
-    <row r="6" spans="2:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="J5" s="10"/>
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="7" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="J6" s="23"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="2:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -711,54 +708,58 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="2:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="L7" s="2"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="2:13" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="J8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>